<commit_message>
planificacion + validacion javascript completa
</commit_message>
<xml_diff>
--- a/PLANIFICACION/PLANIFICACIÓN.xlsx
+++ b/PLANIFICACION/PLANIFICACIÓN.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Planificación</t>
   </si>
@@ -32,7 +32,7 @@
 DE LA TAREA</t>
   </si>
   <si>
-    <t>Abril</t>
+    <t>Mayo</t>
   </si>
   <si>
     <t>SEMANA 1</t>
@@ -41,6 +41,9 @@
     <t>SEMANA 2</t>
   </si>
   <si>
+    <t>SEMANA3</t>
+  </si>
+  <si>
     <t>Quico Sánchez</t>
   </si>
   <si>
@@ -53,12 +56,12 @@
     <t>Mockup Portatil</t>
   </si>
   <si>
+    <t>Creación Login</t>
+  </si>
+  <si>
     <t>Validacion de JavaScript</t>
   </si>
   <si>
-    <t>Creación Login</t>
-  </si>
-  <si>
     <t>Xavi Moreno</t>
   </si>
   <si>
@@ -83,13 +86,16 @@
     <t>Javier Martínez</t>
   </si>
   <si>
-    <t>Creacion Validacion</t>
-  </si>
-  <si>
-    <t>Codigo Login</t>
-  </si>
-  <si>
-    <t>Validacion JS</t>
+    <t>Creación Planificación</t>
+  </si>
+  <si>
+    <t>Mockup Móvil</t>
+  </si>
+  <si>
+    <t>Mockup Portátil</t>
+  </si>
+  <si>
+    <t>Validación JS</t>
   </si>
   <si>
     <t>Gerard Rodríguez</t>
@@ -359,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -405,7 +411,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -478,12 +484,6 @@
     <xf borderId="3" fillId="9" fontId="13" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="0" fillId="8" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -491,9 +491,6 @@
     <xf borderId="4" fillId="7" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="6" fillId="9" fontId="13" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -510,6 +507,9 @@
     <xf borderId="9" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="13" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -524,6 +524,9 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -1197,7 +1200,9 @@
       <c r="O9" s="25"/>
       <c r="P9" s="28"/>
       <c r="Q9" s="30"/>
-      <c r="R9" s="29"/>
+      <c r="R9" s="29" t="s">
+        <v>9</v>
+      </c>
       <c r="S9" s="25"/>
       <c r="T9" s="25"/>
       <c r="U9" s="25"/>
@@ -1258,7 +1263,7 @@
         <v>1.0</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="40"/>
       <c r="D11" s="31"/>
@@ -1336,7 +1341,7 @@
         <v>44927.0</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="43">
         <v>1.0</v>
@@ -1390,7 +1395,7 @@
         <v>44958.0</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="43">
         <v>1.0</v>
@@ -1444,7 +1449,7 @@
         <v>44986.0</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="51">
         <v>1.0</v>
@@ -1458,13 +1463,13 @@
       <c r="J14" s="44"/>
       <c r="K14" s="44"/>
       <c r="L14" s="45"/>
-      <c r="M14" s="44"/>
+      <c r="M14" s="45"/>
       <c r="N14" s="44"/>
-      <c r="O14" s="45"/>
+      <c r="O14" s="44"/>
       <c r="P14" s="44"/>
       <c r="Q14" s="44"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
       <c r="T14" s="44"/>
       <c r="U14" s="46"/>
       <c r="V14" s="2"/>
@@ -1498,7 +1503,7 @@
         <v>45017.0</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="51">
         <v>1.0</v>
@@ -1512,13 +1517,13 @@
       <c r="J15" s="44"/>
       <c r="K15" s="44"/>
       <c r="L15" s="44"/>
-      <c r="M15" s="45"/>
+      <c r="M15" s="44"/>
       <c r="N15" s="45"/>
       <c r="O15" s="45"/>
       <c r="P15" s="44"/>
       <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="44"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
       <c r="T15" s="44"/>
       <c r="U15" s="46"/>
       <c r="V15" s="2"/>
@@ -1552,7 +1557,7 @@
         <v>45047.0</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="51">
         <v>1.0</v>
@@ -1602,31 +1607,57 @@
       <c r="AT16" s="2"/>
     </row>
     <row r="17" ht="15.0" customHeight="1">
-      <c r="A17" s="50">
-        <v>45078.0</v>
-      </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="51">
-        <v>1.0</v>
-      </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="44"/>
-      <c r="T17" s="44"/>
-      <c r="U17" s="46"/>
+      <c r="A17" s="52">
+        <v>2.0</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="32">
+        <v>6.0</v>
+      </c>
+      <c r="F17" s="32">
+        <v>7.0</v>
+      </c>
+      <c r="G17" s="32">
+        <v>8.0</v>
+      </c>
+      <c r="H17" s="32">
+        <v>9.0</v>
+      </c>
+      <c r="I17" s="32">
+        <v>10.0</v>
+      </c>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="32">
+        <v>13.0</v>
+      </c>
+      <c r="M17" s="32">
+        <v>14.0</v>
+      </c>
+      <c r="N17" s="32">
+        <v>15.0</v>
+      </c>
+      <c r="O17" s="32">
+        <v>16.0</v>
+      </c>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="32">
+        <v>21.0</v>
+      </c>
+      <c r="S17" s="32">
+        <v>22.0</v>
+      </c>
+      <c r="T17" s="32">
+        <v>23.0</v>
+      </c>
+      <c r="U17" s="35">
+        <v>24.0</v>
+      </c>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
@@ -1655,30 +1686,32 @@
     </row>
     <row r="18" ht="15.0" customHeight="1">
       <c r="A18" s="50">
-        <v>45108.0</v>
-      </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="51">
+        <v>44928.0</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="55">
         <v>1.0</v>
       </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="53"/>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="46"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+      <c r="S18" s="56"/>
+      <c r="T18" s="56"/>
+      <c r="U18" s="59"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
@@ -1706,111 +1739,87 @@
       <c r="AT18" s="2"/>
     </row>
     <row r="19" ht="15.0" customHeight="1">
-      <c r="A19" s="54">
-        <v>2.0</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="40"/>
+      <c r="A19" s="50">
+        <v>44959.0</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="55">
+        <v>1.0</v>
+      </c>
       <c r="D19" s="56"/>
-      <c r="E19" s="32">
-        <v>6.0</v>
-      </c>
-      <c r="F19" s="32">
-        <v>7.0</v>
-      </c>
-      <c r="G19" s="32">
-        <v>8.0</v>
-      </c>
-      <c r="H19" s="32">
-        <v>9.0</v>
-      </c>
-      <c r="I19" s="32">
-        <v>10.0</v>
-      </c>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="32">
-        <v>13.0</v>
-      </c>
-      <c r="M19" s="32">
-        <v>14.0</v>
-      </c>
-      <c r="N19" s="32">
-        <v>15.0</v>
-      </c>
-      <c r="O19" s="32">
-        <v>16.0</v>
-      </c>
-      <c r="P19" s="34"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="56"/>
+      <c r="P19" s="56"/>
       <c r="Q19" s="56"/>
-      <c r="R19" s="32">
-        <v>21.0</v>
-      </c>
-      <c r="S19" s="32">
-        <v>22.0</v>
-      </c>
-      <c r="T19" s="32">
-        <v>23.0</v>
-      </c>
-      <c r="U19" s="35">
-        <v>24.0</v>
-      </c>
+      <c r="R19" s="56"/>
+      <c r="S19" s="56"/>
+      <c r="T19" s="60"/>
+      <c r="U19" s="59"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="57"/>
-      <c r="X19" s="57"/>
-      <c r="Y19" s="57"/>
+      <c r="W19" s="61"/>
+      <c r="X19" s="61"/>
+      <c r="Y19" s="61"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
-      <c r="AB19" s="57"/>
-      <c r="AC19" s="57"/>
-      <c r="AD19" s="57"/>
+      <c r="AB19" s="61"/>
+      <c r="AC19" s="61"/>
+      <c r="AD19" s="61"/>
       <c r="AE19" s="2"/>
-      <c r="AF19" s="57"/>
-      <c r="AG19" s="57"/>
-      <c r="AH19" s="57"/>
-      <c r="AI19" s="57"/>
-      <c r="AJ19" s="57"/>
-      <c r="AK19" s="57"/>
-      <c r="AL19" s="57"/>
-      <c r="AM19" s="57"/>
-      <c r="AN19" s="57"/>
-      <c r="AO19" s="57"/>
-      <c r="AP19" s="57"/>
-      <c r="AQ19" s="57"/>
-      <c r="AR19" s="57"/>
-      <c r="AS19" s="57"/>
-      <c r="AT19" s="57"/>
+      <c r="AF19" s="61"/>
+      <c r="AG19" s="61"/>
+      <c r="AH19" s="61"/>
+      <c r="AI19" s="61"/>
+      <c r="AJ19" s="61"/>
+      <c r="AK19" s="61"/>
+      <c r="AL19" s="61"/>
+      <c r="AM19" s="61"/>
+      <c r="AN19" s="61"/>
+      <c r="AO19" s="61"/>
+      <c r="AP19" s="61"/>
+      <c r="AQ19" s="61"/>
+      <c r="AR19" s="61"/>
+      <c r="AS19" s="61"/>
+      <c r="AT19" s="61"/>
     </row>
     <row r="20" ht="15.0" customHeight="1">
       <c r="A20" s="50">
-        <v>44928.0</v>
+        <v>44987.0</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="58">
+        <v>18</v>
+      </c>
+      <c r="C20" s="55">
         <v>1.0</v>
       </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="59"/>
-      <c r="R20" s="59"/>
-      <c r="S20" s="59"/>
-      <c r="T20" s="59"/>
-      <c r="U20" s="62"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="56"/>
+      <c r="S20" s="56"/>
+      <c r="T20" s="56"/>
+      <c r="U20" s="59"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
@@ -1839,32 +1848,32 @@
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="A21" s="50">
-        <v>44959.0</v>
+        <v>45018.0</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="58">
+        <v>19</v>
+      </c>
+      <c r="C21" s="55">
         <v>1.0</v>
       </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="59"/>
-      <c r="R21" s="59"/>
-      <c r="S21" s="59"/>
-      <c r="T21" s="63"/>
-      <c r="U21" s="62"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="56"/>
+      <c r="S21" s="56"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="59"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
@@ -1893,32 +1902,32 @@
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="A22" s="50">
-        <v>44987.0</v>
+        <v>45048.0</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="58">
+        <v>20</v>
+      </c>
+      <c r="C22" s="55">
         <v>1.0</v>
       </c>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="59"/>
-      <c r="N22" s="59"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="59"/>
-      <c r="S22" s="59"/>
-      <c r="T22" s="59"/>
-      <c r="U22" s="62"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="56"/>
+      <c r="S22" s="56"/>
+      <c r="T22" s="56"/>
+      <c r="U22" s="59"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
@@ -1947,32 +1956,32 @@
     </row>
     <row r="23" ht="15.0" customHeight="1">
       <c r="A23" s="50">
-        <v>45018.0</v>
+        <v>45079.0</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="58">
+        <v>21</v>
+      </c>
+      <c r="C23" s="55">
         <v>1.0</v>
       </c>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="59"/>
-      <c r="T23" s="59"/>
-      <c r="U23" s="62"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="59"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
@@ -2001,32 +2010,31 @@
     </row>
     <row r="24" ht="15.0" customHeight="1">
       <c r="A24" s="50">
-        <v>45048.0</v>
+        <v>45109.0</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="58">
+        <v>22</v>
+      </c>
+      <c r="C24" s="55">
         <v>1.0</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="59"/>
-      <c r="R24" s="59"/>
-      <c r="S24" s="59"/>
-      <c r="T24" s="59"/>
-      <c r="U24" s="62"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="56"/>
+      <c r="P24" s="56"/>
+      <c r="Q24" s="56"/>
+      <c r="R24" s="56"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
@@ -2054,33 +2062,57 @@
       <c r="AT24" s="2"/>
     </row>
     <row r="25" ht="15.0" customHeight="1">
-      <c r="A25" s="50">
-        <v>45079.0</v>
-      </c>
-      <c r="B25" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="58">
-        <v>1.0</v>
-      </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="59"/>
-      <c r="U25" s="62"/>
+      <c r="A25" s="52">
+        <v>3.0</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="32">
+        <v>6.0</v>
+      </c>
+      <c r="F25" s="32">
+        <v>7.0</v>
+      </c>
+      <c r="G25" s="32">
+        <v>8.0</v>
+      </c>
+      <c r="H25" s="32">
+        <v>9.0</v>
+      </c>
+      <c r="I25" s="32">
+        <v>10.0</v>
+      </c>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="32">
+        <v>13.0</v>
+      </c>
+      <c r="M25" s="32">
+        <v>14.0</v>
+      </c>
+      <c r="N25" s="32">
+        <v>15.0</v>
+      </c>
+      <c r="O25" s="32">
+        <v>16.0</v>
+      </c>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="32">
+        <v>21.0</v>
+      </c>
+      <c r="S25" s="32">
+        <v>22.0</v>
+      </c>
+      <c r="T25" s="32">
+        <v>23.0</v>
+      </c>
+      <c r="U25" s="35">
+        <v>24.0</v>
+      </c>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
@@ -2108,33 +2140,33 @@
       <c r="AT25" s="2"/>
     </row>
     <row r="26" ht="15.0" customHeight="1">
-      <c r="A26" s="50">
-        <v>45109.0</v>
+      <c r="A26" s="62">
+        <v>44929.0</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="58">
+        <v>24</v>
+      </c>
+      <c r="C26" s="63">
         <v>1.0</v>
       </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="60"/>
-      <c r="U26" s="60"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="49"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
@@ -2162,103 +2194,79 @@
       <c r="AT26" s="2"/>
     </row>
     <row r="27" ht="15.0" customHeight="1">
-      <c r="A27" s="54">
-        <v>3.0</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="32">
-        <v>6.0</v>
-      </c>
-      <c r="F27" s="32">
-        <v>7.0</v>
-      </c>
-      <c r="G27" s="32">
-        <v>8.0</v>
-      </c>
-      <c r="H27" s="32">
-        <v>9.0</v>
-      </c>
-      <c r="I27" s="32">
-        <v>10.0</v>
-      </c>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="32">
-        <v>13.0</v>
-      </c>
-      <c r="M27" s="32">
-        <v>14.0</v>
-      </c>
-      <c r="N27" s="32">
-        <v>15.0</v>
-      </c>
-      <c r="O27" s="32">
-        <v>16.0</v>
-      </c>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="32">
-        <v>21.0</v>
-      </c>
-      <c r="S27" s="32">
-        <v>22.0</v>
-      </c>
-      <c r="T27" s="32">
-        <v>23.0</v>
-      </c>
-      <c r="U27" s="35">
-        <v>24.0</v>
-      </c>
+      <c r="A27" s="62">
+        <v>44960.0</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="63">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="49"/>
       <c r="V27" s="2"/>
-      <c r="W27" s="57"/>
-      <c r="X27" s="57"/>
-      <c r="Y27" s="57"/>
+      <c r="W27" s="61"/>
+      <c r="X27" s="61"/>
+      <c r="Y27" s="61"/>
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
-      <c r="AB27" s="57"/>
-      <c r="AC27" s="57"/>
-      <c r="AD27" s="57"/>
+      <c r="AB27" s="61"/>
+      <c r="AC27" s="61"/>
+      <c r="AD27" s="61"/>
       <c r="AE27" s="2"/>
-      <c r="AF27" s="57"/>
-      <c r="AG27" s="57"/>
-      <c r="AH27" s="57"/>
-      <c r="AI27" s="57"/>
-      <c r="AJ27" s="57"/>
-      <c r="AK27" s="57"/>
-      <c r="AL27" s="57"/>
-      <c r="AM27" s="57"/>
-      <c r="AN27" s="57"/>
-      <c r="AO27" s="57"/>
-      <c r="AP27" s="57"/>
-      <c r="AQ27" s="57"/>
-      <c r="AR27" s="57"/>
-      <c r="AS27" s="57"/>
-      <c r="AT27" s="57"/>
+      <c r="AF27" s="61"/>
+      <c r="AG27" s="61"/>
+      <c r="AH27" s="61"/>
+      <c r="AI27" s="61"/>
+      <c r="AJ27" s="61"/>
+      <c r="AK27" s="61"/>
+      <c r="AL27" s="61"/>
+      <c r="AM27" s="61"/>
+      <c r="AN27" s="61"/>
+      <c r="AO27" s="61"/>
+      <c r="AP27" s="61"/>
+      <c r="AQ27" s="61"/>
+      <c r="AR27" s="61"/>
+      <c r="AS27" s="61"/>
+      <c r="AT27" s="61"/>
     </row>
     <row r="28" ht="15.0" customHeight="1">
-      <c r="A28" s="64">
-        <v>44929.0</v>
+      <c r="A28" s="62">
+        <v>44988.0</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="65">
+        <v>26</v>
+      </c>
+      <c r="C28" s="63">
         <v>1.0</v>
       </c>
       <c r="D28" s="44"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
       <c r="G28" s="44"/>
       <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
+      <c r="I28" s="45"/>
       <c r="J28" s="44"/>
       <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
       <c r="N28" s="44"/>
       <c r="O28" s="44"/>
       <c r="P28" s="44"/>
@@ -2294,27 +2302,27 @@
       <c r="AT28" s="2"/>
     </row>
     <row r="29" ht="15.0" customHeight="1">
-      <c r="A29" s="64">
-        <v>44960.0</v>
+      <c r="A29" s="62">
+        <v>45019.0</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="65">
+        <v>14</v>
+      </c>
+      <c r="C29" s="63">
         <v>1.0</v>
       </c>
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
       <c r="I29" s="44"/>
       <c r="J29" s="44"/>
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
       <c r="P29" s="44"/>
       <c r="Q29" s="44"/>
       <c r="R29" s="44"/>
@@ -2348,31 +2356,31 @@
       <c r="AT29" s="2"/>
     </row>
     <row r="30" ht="15.0" customHeight="1">
-      <c r="A30" s="64">
-        <v>44988.0</v>
-      </c>
-      <c r="B30" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="65">
+      <c r="A30" s="62">
+        <v>45049.0</v>
+      </c>
+      <c r="B30" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="63">
         <v>1.0</v>
       </c>
-      <c r="D30" s="44"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="44"/>
       <c r="F30" s="44"/>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
-      <c r="I30" s="45"/>
+      <c r="I30" s="44"/>
       <c r="J30" s="44"/>
       <c r="K30" s="44"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44"/>
       <c r="N30" s="44"/>
       <c r="O30" s="44"/>
       <c r="P30" s="44"/>
       <c r="Q30" s="44"/>
-      <c r="R30" s="44"/>
-      <c r="S30" s="44"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
       <c r="T30" s="44"/>
       <c r="U30" s="49"/>
       <c r="V30" s="2"/>
@@ -2402,33 +2410,57 @@
       <c r="AT30" s="2"/>
     </row>
     <row r="31" ht="15.0" customHeight="1">
-      <c r="A31" s="64">
-        <v>45019.0</v>
-      </c>
-      <c r="B31" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="65">
-        <v>1.0</v>
-      </c>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="44"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="44"/>
-      <c r="S31" s="44"/>
-      <c r="T31" s="44"/>
-      <c r="U31" s="49"/>
+      <c r="A31" s="52">
+        <v>4.0</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="40"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="32">
+        <v>6.0</v>
+      </c>
+      <c r="F31" s="32">
+        <v>7.0</v>
+      </c>
+      <c r="G31" s="32">
+        <v>8.0</v>
+      </c>
+      <c r="H31" s="32">
+        <v>9.0</v>
+      </c>
+      <c r="I31" s="32">
+        <v>10.0</v>
+      </c>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="32">
+        <v>13.0</v>
+      </c>
+      <c r="M31" s="32">
+        <v>14.0</v>
+      </c>
+      <c r="N31" s="32">
+        <v>15.0</v>
+      </c>
+      <c r="O31" s="32">
+        <v>16.0</v>
+      </c>
+      <c r="P31" s="34"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="32">
+        <v>21.0</v>
+      </c>
+      <c r="S31" s="32">
+        <v>22.0</v>
+      </c>
+      <c r="T31" s="32">
+        <v>23.0</v>
+      </c>
+      <c r="U31" s="35">
+        <v>24.0</v>
+      </c>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
@@ -2456,33 +2488,33 @@
       <c r="AT31" s="2"/>
     </row>
     <row r="32" ht="15.0" customHeight="1">
-      <c r="A32" s="64">
-        <v>45049.0</v>
-      </c>
-      <c r="B32" s="66" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="65">
+      <c r="A32" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="51">
         <v>1.0</v>
       </c>
       <c r="D32" s="67"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="44"/>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="44"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="45"/>
-      <c r="U32" s="49"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67"/>
+      <c r="O32" s="67"/>
+      <c r="P32" s="67"/>
+      <c r="Q32" s="67"/>
+      <c r="R32" s="67"/>
+      <c r="S32" s="67"/>
+      <c r="T32" s="67"/>
+      <c r="U32" s="46"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
@@ -2510,57 +2542,33 @@
       <c r="AT32" s="2"/>
     </row>
     <row r="33" ht="15.0" customHeight="1">
-      <c r="A33" s="54">
-        <v>4.0</v>
-      </c>
-      <c r="B33" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="32">
-        <v>6.0</v>
-      </c>
-      <c r="F33" s="32">
-        <v>7.0</v>
-      </c>
-      <c r="G33" s="32">
-        <v>8.0</v>
-      </c>
-      <c r="H33" s="32">
-        <v>9.0</v>
-      </c>
-      <c r="I33" s="32">
-        <v>10.0</v>
-      </c>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="32">
-        <v>13.0</v>
-      </c>
-      <c r="M33" s="32">
-        <v>14.0</v>
-      </c>
-      <c r="N33" s="32">
-        <v>15.0</v>
-      </c>
-      <c r="O33" s="32">
-        <v>16.0</v>
-      </c>
-      <c r="P33" s="34"/>
-      <c r="Q33" s="56"/>
-      <c r="R33" s="32">
-        <v>21.0</v>
-      </c>
-      <c r="S33" s="32">
-        <v>22.0</v>
-      </c>
-      <c r="T33" s="32">
-        <v>23.0</v>
-      </c>
-      <c r="U33" s="35">
-        <v>24.0</v>
-      </c>
+      <c r="A33" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="51">
+        <v>1.0</v>
+      </c>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="67"/>
+      <c r="N33" s="67"/>
+      <c r="O33" s="67"/>
+      <c r="P33" s="67"/>
+      <c r="Q33" s="67"/>
+      <c r="R33" s="67"/>
+      <c r="S33" s="67"/>
+      <c r="T33" s="67"/>
+      <c r="U33" s="46"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
       <c r="X33" s="2"/>
@@ -2588,32 +2596,32 @@
       <c r="AT33" s="2"/>
     </row>
     <row r="34" ht="15.0" customHeight="1">
-      <c r="A34" s="68" t="s">
-        <v>27</v>
+      <c r="A34" s="66" t="s">
+        <v>32</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C34" s="51">
         <v>1.0</v>
       </c>
-      <c r="D34" s="53"/>
-      <c r="E34" s="45"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
       <c r="F34" s="45"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="53"/>
-      <c r="N34" s="53"/>
-      <c r="O34" s="53"/>
-      <c r="P34" s="53"/>
-      <c r="Q34" s="53"/>
-      <c r="R34" s="53"/>
-      <c r="S34" s="53"/>
-      <c r="T34" s="53"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="67"/>
+      <c r="P34" s="67"/>
+      <c r="Q34" s="67"/>
+      <c r="R34" s="67"/>
+      <c r="S34" s="67"/>
+      <c r="T34" s="67"/>
       <c r="U34" s="46"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
@@ -2642,32 +2650,32 @@
       <c r="AT34" s="2"/>
     </row>
     <row r="35" ht="15.0" customHeight="1">
-      <c r="A35" s="68" t="s">
-        <v>29</v>
+      <c r="A35" s="66" t="s">
+        <v>34</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C35" s="51">
         <v>1.0</v>
       </c>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="53"/>
-      <c r="P35" s="53"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="53"/>
-      <c r="S35" s="53"/>
-      <c r="T35" s="53"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="67"/>
+      <c r="N35" s="67"/>
+      <c r="O35" s="67"/>
+      <c r="P35" s="67"/>
+      <c r="Q35" s="67"/>
+      <c r="R35" s="67"/>
+      <c r="S35" s="67"/>
+      <c r="T35" s="67"/>
       <c r="U35" s="46"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
@@ -2696,32 +2704,32 @@
       <c r="AT35" s="2"/>
     </row>
     <row r="36" ht="15.0" customHeight="1">
-      <c r="A36" s="68" t="s">
-        <v>30</v>
+      <c r="A36" s="66" t="s">
+        <v>36</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="51">
+        <v>18</v>
+      </c>
+      <c r="C36" s="43">
         <v>1.0</v>
       </c>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="53"/>
-      <c r="N36" s="53"/>
-      <c r="O36" s="53"/>
-      <c r="P36" s="53"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="53"/>
-      <c r="S36" s="53"/>
-      <c r="T36" s="53"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="45"/>
+      <c r="N36" s="71"/>
+      <c r="O36" s="71"/>
+      <c r="P36" s="67"/>
+      <c r="Q36" s="67"/>
+      <c r="R36" s="67"/>
+      <c r="S36" s="67"/>
+      <c r="T36" s="67"/>
       <c r="U36" s="46"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
@@ -2750,32 +2758,32 @@
       <c r="AT36" s="2"/>
     </row>
     <row r="37" ht="15.0" customHeight="1">
-      <c r="A37" s="68" t="s">
-        <v>32</v>
+      <c r="A37" s="66" t="s">
+        <v>37</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="51">
+        <v>38</v>
+      </c>
+      <c r="C37" s="43">
         <v>1.0</v>
       </c>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
-      <c r="O37" s="53"/>
-      <c r="P37" s="53"/>
-      <c r="Q37" s="53"/>
-      <c r="R37" s="53"/>
-      <c r="S37" s="53"/>
-      <c r="T37" s="53"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="67"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="67"/>
+      <c r="Q37" s="67"/>
+      <c r="R37" s="71"/>
+      <c r="S37" s="71"/>
+      <c r="T37" s="67"/>
       <c r="U37" s="46"/>
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
@@ -2804,33 +2812,31 @@
       <c r="AT37" s="2"/>
     </row>
     <row r="38" ht="15.0" customHeight="1">
-      <c r="A38" s="68" t="s">
-        <v>34</v>
+      <c r="A38" s="66" t="s">
+        <v>39</v>
       </c>
       <c r="B38" s="42" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C38" s="43">
         <v>1.0</v>
       </c>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="72"/>
-      <c r="O38" s="72"/>
-      <c r="P38" s="53"/>
-      <c r="Q38" s="53"/>
-      <c r="R38" s="53"/>
-      <c r="S38" s="53"/>
-      <c r="T38" s="53"/>
-      <c r="U38" s="46"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="61"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="61"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="61"/>
+      <c r="O38" s="61"/>
+      <c r="P38" s="61"/>
+      <c r="Q38" s="61"/>
+      <c r="R38" s="72"/>
+      <c r="S38" s="72"/>
+      <c r="T38" s="61"/>
+      <c r="U38" s="61"/>
       <c r="V38" s="2"/>
       <c r="W38" s="2"/>
       <c r="X38" s="2"/>
@@ -2858,33 +2864,6 @@
       <c r="AT38" s="2"/>
     </row>
     <row r="39" ht="15.0" customHeight="1">
-      <c r="A39" s="68" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="43">
-        <v>1.0</v>
-      </c>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="53"/>
-      <c r="Q39" s="53"/>
-      <c r="R39" s="72"/>
-      <c r="S39" s="72"/>
-      <c r="T39" s="53"/>
-      <c r="U39" s="46"/>
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
       <c r="X39" s="2"/>
@@ -2912,56 +2891,31 @@
       <c r="AT39" s="2"/>
     </row>
     <row r="40" ht="15.0" customHeight="1">
-      <c r="A40" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="43">
-        <v>1.0</v>
-      </c>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="57"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="57"/>
-      <c r="M40" s="57"/>
-      <c r="N40" s="57"/>
-      <c r="O40" s="57"/>
-      <c r="P40" s="57"/>
-      <c r="Q40" s="57"/>
-      <c r="R40" s="73"/>
-      <c r="S40" s="73"/>
-      <c r="T40" s="57"/>
-      <c r="U40" s="57"/>
-      <c r="V40" s="57"/>
-      <c r="W40" s="57"/>
-      <c r="X40" s="57"/>
-      <c r="Y40" s="57"/>
+      <c r="V40" s="61"/>
+      <c r="W40" s="61"/>
+      <c r="X40" s="61"/>
+      <c r="Y40" s="61"/>
       <c r="Z40" s="2"/>
       <c r="AA40" s="2"/>
-      <c r="AB40" s="57"/>
-      <c r="AC40" s="57"/>
-      <c r="AD40" s="57"/>
+      <c r="AB40" s="61"/>
+      <c r="AC40" s="61"/>
+      <c r="AD40" s="61"/>
       <c r="AE40" s="2"/>
-      <c r="AF40" s="57"/>
-      <c r="AG40" s="57"/>
-      <c r="AH40" s="57"/>
-      <c r="AI40" s="57"/>
-      <c r="AJ40" s="57"/>
-      <c r="AK40" s="57"/>
-      <c r="AL40" s="57"/>
-      <c r="AM40" s="57"/>
-      <c r="AN40" s="57"/>
-      <c r="AO40" s="57"/>
-      <c r="AP40" s="57"/>
-      <c r="AQ40" s="57"/>
-      <c r="AR40" s="57"/>
-      <c r="AS40" s="57"/>
-      <c r="AT40" s="57"/>
+      <c r="AF40" s="61"/>
+      <c r="AG40" s="61"/>
+      <c r="AH40" s="61"/>
+      <c r="AI40" s="61"/>
+      <c r="AJ40" s="61"/>
+      <c r="AK40" s="61"/>
+      <c r="AL40" s="61"/>
+      <c r="AM40" s="61"/>
+      <c r="AN40" s="61"/>
+      <c r="AO40" s="61"/>
+      <c r="AP40" s="61"/>
+      <c r="AQ40" s="61"/>
+      <c r="AR40" s="61"/>
+      <c r="AS40" s="61"/>
+      <c r="AT40" s="61"/>
     </row>
     <row r="41" ht="15.0" customHeight="1">
       <c r="F41" s="2"/>
@@ -3205,49 +3159,49 @@
       <c r="AT46" s="2"/>
     </row>
     <row r="49">
-      <c r="B49" s="74"/>
+      <c r="B49" s="73"/>
     </row>
     <row r="50">
-      <c r="B50" s="74"/>
+      <c r="B50" s="73"/>
     </row>
     <row r="51">
-      <c r="B51" s="75"/>
+      <c r="B51" s="74"/>
     </row>
     <row r="52">
-      <c r="B52" s="76"/>
+      <c r="B52" s="75"/>
     </row>
     <row r="53">
-      <c r="B53" s="74"/>
+      <c r="B53" s="73"/>
     </row>
     <row r="54">
-      <c r="B54" s="74"/>
+      <c r="B54" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="24">
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="H2:M2"/>
+    <mergeCell ref="N2:AG2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="H4:N4"/>
-    <mergeCell ref="N2:AG2"/>
     <mergeCell ref="O4:Y4"/>
+    <mergeCell ref="D8:U8"/>
+    <mergeCell ref="V8:AR8"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="L9:O9"/>
     <mergeCell ref="V9:Z9"/>
     <mergeCell ref="AA9:AE9"/>
     <mergeCell ref="AF9:AJ9"/>
     <mergeCell ref="AK9:AO9"/>
     <mergeCell ref="AP9:AT9"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="V8:AR8"/>
-    <mergeCell ref="E9:I9"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="H5:N5"/>
+    <mergeCell ref="O5:X5"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:U8"/>
-    <mergeCell ref="O5:X5"/>
-    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="R9:U9"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>